<commit_message>
wp. another way of compiling stacked horizontal bar chart
</commit_message>
<xml_diff>
--- a/tests/resources/horizontal_bar_chart_manual_data.xlsx
+++ b/tests/resources/horizontal_bar_chart_manual_data.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">SRO ratings</t>
   </si>
   <si>
     <t xml:space="preserve">Q4 20/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3 20/21</t>
   </si>
   <si>
     <t xml:space="preserve">Green</t>
@@ -148,7 +151,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -160,67 +163,81 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0.0395157490054331</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.0328776917232356</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.0689255597551642</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0.0183568800324753</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.0316495964211099</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.0281620223943915</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.352632446856195</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.368860776116387</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.327944919102807</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>0.333640099505067</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.321790376457074</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.26121648412432</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.238105667322601</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.240338889719215</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.313751014623316</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>0.0177491572782287</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.00448266956297767</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>